<commit_message>
chore: generate Jekyll collections from Excel
</commit_message>
<xml_diff>
--- a/data/luismcsoul_content_export.xlsx
+++ b/data/luismcsoul_content_export.xlsx
@@ -6937,7 +6937,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t xml:space="preserve">ARMORED HEART
+          <t>ARMORED HEART
 If you were hurt,
 it's natural for you to close
 your doors/a practical distrust,
@@ -6950,8 +6950,7 @@
 I'm sorry you meet me in decadence.
 There's not only one version of ourselves,
 I'm sorry you meet this creepy and lame:
-Armored Heart
-</t>
+Armored Heart</t>
         </is>
       </c>
     </row>

</xml_diff>